<commit_message>
Added VolumeScan and PointCloud, to support X-ray centring (etc.) First Draft.
</commit_message>
<xml_diff>
--- a/docs/examples/mapping_0.6.7_preliminary.xlsx
+++ b/docs/examples/mapping_0.6.7_preliminary.xlsx
@@ -1141,6 +1141,9 @@
     <t xml:space="preserve">Oscillation Range</t>
   </si>
   <si>
+    <t xml:space="preserve">min osc. angle</t>
+  </si>
+  <si>
     <t xml:space="preserve">CollectionSweep.numberImages</t>
   </si>
   <si>
@@ -1724,9 +1727,6 @@
   </si>
   <si>
     <t xml:space="preserve">Directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min osc. angle</t>
   </si>
   <si>
     <t xml:space="preserve">proposalCode</t>
@@ -2021,7 +2021,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2058,16 +2058,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -2217,11 +2213,11 @@
   <dimension ref="A1:Z263"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H119" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
-      <selection pane="bottomRight" activeCell="Z30" activeCellId="0" sqref="Z30"/>
+      <selection pane="bottomLeft" activeCell="A119" activeCellId="0" sqref="A119"/>
+      <selection pane="bottomRight" activeCell="X142" activeCellId="0" sqref="X142:Y142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -3198,7 +3194,7 @@
       <c r="Y30" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="Z30" s="9" t="s">
+      <c r="Z30" s="6" t="s">
         <v>89</v>
       </c>
     </row>
@@ -6883,7 +6879,12 @@
       <c r="W142" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="X142" s="7"/>
+      <c r="X142" s="7" t="n">
+        <v>26</v>
+      </c>
+      <c r="Y142" s="2" t="s">
+        <v>344</v>
+      </c>
       <c r="Z142" s="8"/>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
@@ -6891,13 +6892,13 @@
         <v>142</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="E143" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H143" s="7"/>
       <c r="K143" s="8"/>
@@ -6917,13 +6918,13 @@
         <v>143</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="H144" s="7"/>
       <c r="K144" s="8"/>
@@ -6943,13 +6944,13 @@
         <v>144</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H145" s="7"/>
       <c r="K145" s="8"/>
@@ -6969,13 +6970,13 @@
         <v>145</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="H146" s="7"/>
       <c r="K146" s="8"/>
@@ -6995,13 +6996,13 @@
         <v>146</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H147" s="7"/>
       <c r="K147" s="8"/>
@@ -7021,13 +7022,13 @@
         <v>147</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="H148" s="7"/>
       <c r="K148" s="8"/>
@@ -7047,13 +7048,13 @@
         <v>148</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="H149" s="7"/>
       <c r="K149" s="8"/>
@@ -7061,7 +7062,7 @@
         <v>29</v>
       </c>
       <c r="M149" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="N149" s="8"/>
       <c r="O149" s="7"/>
@@ -7070,7 +7071,7 @@
         <v>29</v>
       </c>
       <c r="S149" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="T149" s="8"/>
       <c r="U149" s="7"/>
@@ -7083,13 +7084,13 @@
         <v>149</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="E150" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="H150" s="7" t="n">
         <v>15</v>
@@ -7098,14 +7099,14 @@
         <v>231</v>
       </c>
       <c r="J150" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K150" s="8"/>
       <c r="L150" s="7" t="n">
         <v>30</v>
       </c>
       <c r="M150" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N150" s="8"/>
       <c r="O150" s="7"/>
@@ -7122,13 +7123,13 @@
         <v>150</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E151" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="H151" s="7"/>
       <c r="K151" s="8"/>
@@ -7136,7 +7137,7 @@
         <v>27</v>
       </c>
       <c r="M151" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N151" s="8" t="s">
         <v>131</v>
@@ -7151,7 +7152,7 @@
         <v>27</v>
       </c>
       <c r="Y151" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="Z151" s="8" t="s">
         <v>131</v>
@@ -7162,13 +7163,13 @@
         <v>151</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H152" s="7"/>
       <c r="K152" s="8"/>
@@ -7188,13 +7189,13 @@
         <v>152</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="H153" s="7"/>
       <c r="K153" s="8"/>
@@ -7214,13 +7215,13 @@
         <v>153</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H154" s="7"/>
       <c r="K154" s="8"/>
@@ -7228,10 +7229,10 @@
         <v>18</v>
       </c>
       <c r="M154" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="N154" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="O154" s="7"/>
       <c r="Q154" s="8"/>
@@ -7243,10 +7244,10 @@
         <v>18</v>
       </c>
       <c r="Y154" s="2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="Z154" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
@@ -7254,13 +7255,13 @@
         <v>154</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H155" s="7"/>
       <c r="K155" s="8"/>
@@ -7280,13 +7281,13 @@
         <v>155</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H156" s="7"/>
       <c r="K156" s="8"/>
@@ -7306,13 +7307,13 @@
         <v>156</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H157" s="7"/>
       <c r="K157" s="8"/>
@@ -7327,56 +7328,76 @@
       <c r="X157" s="7"/>
       <c r="Z157" s="8"/>
     </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="158" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A158" s="1" t="n">
         <v>157</v>
       </c>
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
       <c r="D158" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>382</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="G158" s="2"/>
       <c r="H158" s="7"/>
+      <c r="I158" s="2"/>
+      <c r="J158" s="2"/>
       <c r="K158" s="8"/>
       <c r="L158" s="7"/>
+      <c r="M158" s="2"/>
       <c r="N158" s="8"/>
       <c r="O158" s="7"/>
+      <c r="P158" s="2"/>
       <c r="Q158" s="8"/>
       <c r="R158" s="7"/>
+      <c r="S158" s="2"/>
       <c r="T158" s="8"/>
       <c r="U158" s="7"/>
+      <c r="V158" s="2"/>
       <c r="W158" s="8"/>
       <c r="X158" s="7"/>
+      <c r="Y158" s="2"/>
       <c r="Z158" s="8"/>
     </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="159" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A159" s="1" t="n">
         <v>158</v>
       </c>
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
       <c r="D159" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>384</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="G159" s="2"/>
       <c r="H159" s="7"/>
+      <c r="I159" s="2"/>
+      <c r="J159" s="2"/>
       <c r="K159" s="8"/>
       <c r="L159" s="7"/>
+      <c r="M159" s="2"/>
       <c r="N159" s="8"/>
       <c r="O159" s="7"/>
+      <c r="P159" s="2"/>
       <c r="Q159" s="8"/>
       <c r="R159" s="7"/>
+      <c r="S159" s="2"/>
       <c r="T159" s="8"/>
       <c r="U159" s="7"/>
+      <c r="V159" s="2"/>
       <c r="W159" s="8"/>
       <c r="X159" s="7"/>
+      <c r="Y159" s="2"/>
       <c r="Z159" s="8"/>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
@@ -7384,13 +7405,13 @@
         <v>159</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H160" s="7"/>
       <c r="K160" s="8"/>
@@ -7410,13 +7431,13 @@
         <v>160</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H161" s="7"/>
       <c r="K161" s="8"/>
@@ -7436,13 +7457,13 @@
         <v>161</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H162" s="7"/>
       <c r="K162" s="8"/>
@@ -7462,13 +7483,13 @@
         <v>162</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H163" s="7"/>
       <c r="K163" s="8"/>
@@ -7488,13 +7509,13 @@
         <v>163</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="H164" s="7"/>
       <c r="K164" s="8"/>
@@ -7514,13 +7535,13 @@
         <v>164</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H165" s="7"/>
       <c r="K165" s="8"/>
@@ -7543,10 +7564,10 @@
         <v>218</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="H166" s="7"/>
       <c r="K166" s="8"/>
@@ -7592,7 +7613,7 @@
         <v>167</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>23</v>
@@ -7618,7 +7639,7 @@
         <v>168</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="E169" s="2" t="s">
         <v>23</v>
@@ -7644,7 +7665,7 @@
         <v>169</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="E170" s="2" t="s">
         <v>227</v>
@@ -7670,13 +7691,13 @@
         <v>170</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H171" s="7" t="n">
         <v>18</v>
@@ -7685,7 +7706,7 @@
         <v>85</v>
       </c>
       <c r="J171" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="K171" s="8"/>
       <c r="L171" s="7"/>
@@ -7704,13 +7725,13 @@
         <v>171</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E172" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H172" s="7"/>
       <c r="K172" s="8"/>
@@ -7730,13 +7751,13 @@
         <v>172</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E173" s="2" t="s">
         <v>279</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="H173" s="7"/>
       <c r="K173" s="8"/>
@@ -7744,7 +7765,7 @@
         <v>22</v>
       </c>
       <c r="M173" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="N173" s="8"/>
       <c r="O173" s="7"/>
@@ -7757,7 +7778,7 @@
         <v>22</v>
       </c>
       <c r="Y173" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="Z173" s="8"/>
     </row>
@@ -7766,7 +7787,7 @@
         <v>173</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E174" s="2" t="s">
         <v>158</v>
@@ -7792,7 +7813,7 @@
         <v>174</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E175" s="2" t="s">
         <v>158</v>
@@ -7818,7 +7839,7 @@
         <v>175</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="E176" s="2" t="s">
         <v>158</v>
@@ -7844,7 +7865,7 @@
         <v>176</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E177" s="2" t="s">
         <v>158</v>
@@ -7870,7 +7891,7 @@
         <v>177</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="E178" s="2" t="s">
         <v>158</v>
@@ -7896,7 +7917,7 @@
         <v>178</v>
       </c>
       <c r="D179" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E179" s="2" t="s">
         <v>158</v>
@@ -7925,10 +7946,10 @@
         <v>326</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H180" s="7"/>
       <c r="K180" s="8"/>
@@ -7974,7 +7995,7 @@
         <v>181</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>23</v>
@@ -8000,13 +8021,13 @@
         <v>182</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H183" s="7"/>
       <c r="K183" s="8"/>
@@ -8026,13 +8047,13 @@
         <v>183</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E184" s="2" t="s">
         <v>279</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H184" s="7"/>
       <c r="K184" s="8"/>
@@ -8052,7 +8073,7 @@
         <v>184</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="E185" s="2" t="s">
         <v>158</v>
@@ -8078,7 +8099,7 @@
         <v>185</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="E186" s="2" t="s">
         <v>158</v>
@@ -8104,7 +8125,7 @@
         <v>186</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="E187" s="2" t="s">
         <v>158</v>
@@ -8130,7 +8151,7 @@
         <v>187</v>
       </c>
       <c r="D188" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E188" s="2" t="s">
         <v>158</v>
@@ -8156,7 +8177,7 @@
         <v>188</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E189" s="2" t="s">
         <v>158</v>
@@ -8182,7 +8203,7 @@
         <v>189</v>
       </c>
       <c r="D190" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E190" s="2" t="s">
         <v>158</v>
@@ -8208,13 +8229,13 @@
         <v>190</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="E191" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H191" s="7"/>
       <c r="K191" s="8"/>
@@ -8234,13 +8255,13 @@
         <v>191</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H192" s="7"/>
       <c r="K192" s="8"/>
@@ -8260,13 +8281,13 @@
         <v>192</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F193" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H193" s="7"/>
       <c r="K193" s="8"/>
@@ -8286,13 +8307,13 @@
         <v>193</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F194" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H194" s="7"/>
       <c r="K194" s="8"/>
@@ -8312,13 +8333,13 @@
         <v>194</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E195" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F195" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H195" s="7"/>
       <c r="K195" s="8"/>
@@ -8338,13 +8359,13 @@
         <v>195</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H196" s="7"/>
       <c r="K196" s="8"/>
@@ -8364,13 +8385,13 @@
         <v>196</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F197" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H197" s="7"/>
       <c r="K197" s="8"/>
@@ -8390,13 +8411,13 @@
         <v>197</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="E198" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H198" s="7"/>
       <c r="K198" s="8"/>
@@ -8416,13 +8437,13 @@
         <v>198</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="E199" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F199" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H199" s="7"/>
       <c r="K199" s="8"/>
@@ -8442,13 +8463,13 @@
         <v>199</v>
       </c>
       <c r="D200" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F200" s="2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H200" s="7"/>
       <c r="K200" s="8"/>
@@ -8468,13 +8489,13 @@
         <v>200</v>
       </c>
       <c r="D201" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F201" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H201" s="7"/>
       <c r="K201" s="8"/>
@@ -8494,13 +8515,13 @@
         <v>201</v>
       </c>
       <c r="D202" s="2" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F202" s="2" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H202" s="7"/>
       <c r="K202" s="8"/>
@@ -8520,13 +8541,13 @@
         <v>202</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F203" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H203" s="7"/>
       <c r="K203" s="8"/>
@@ -8546,13 +8567,13 @@
         <v>203</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E204" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F204" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H204" s="7"/>
       <c r="K204" s="8"/>
@@ -8572,13 +8593,13 @@
         <v>204</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="E205" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F205" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="H205" s="7"/>
       <c r="K205" s="8"/>
@@ -8598,13 +8619,13 @@
         <v>205</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E206" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F206" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="H206" s="7"/>
       <c r="K206" s="8"/>
@@ -8624,13 +8645,13 @@
         <v>206</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="E207" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F207" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="H207" s="7"/>
       <c r="K207" s="8"/>
@@ -8650,13 +8671,13 @@
         <v>207</v>
       </c>
       <c r="D208" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E208" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F208" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="H208" s="7"/>
       <c r="K208" s="8"/>
@@ -8676,13 +8697,13 @@
         <v>208</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E209" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F209" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="H209" s="7"/>
       <c r="K209" s="8"/>
@@ -8702,13 +8723,13 @@
         <v>209</v>
       </c>
       <c r="D210" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="E210" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F210" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="H210" s="7"/>
       <c r="K210" s="8"/>
@@ -8728,13 +8749,13 @@
         <v>210</v>
       </c>
       <c r="D211" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E211" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F211" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="H211" s="7"/>
       <c r="K211" s="8"/>
@@ -8754,13 +8775,13 @@
         <v>211</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E212" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F212" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H212" s="7"/>
       <c r="K212" s="8"/>
@@ -8780,13 +8801,13 @@
         <v>212</v>
       </c>
       <c r="D213" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E213" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F213" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H213" s="7"/>
       <c r="K213" s="8"/>
@@ -8806,13 +8827,13 @@
         <v>213</v>
       </c>
       <c r="D214" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E214" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F214" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H214" s="7"/>
       <c r="K214" s="8"/>
@@ -8832,13 +8853,13 @@
         <v>214</v>
       </c>
       <c r="D215" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="E215" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F215" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H215" s="7"/>
       <c r="K215" s="8"/>
@@ -8858,13 +8879,13 @@
         <v>215</v>
       </c>
       <c r="D216" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E216" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F216" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H216" s="7"/>
       <c r="K216" s="8"/>
@@ -8884,13 +8905,13 @@
         <v>216</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="E217" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F217" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="H217" s="7"/>
       <c r="K217" s="8"/>
@@ -8910,13 +8931,13 @@
         <v>217</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E218" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F218" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="H218" s="7"/>
       <c r="K218" s="8"/>
@@ -8936,13 +8957,13 @@
         <v>218</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E219" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F219" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="H219" s="7"/>
       <c r="K219" s="8"/>
@@ -8962,13 +8983,13 @@
         <v>219</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E220" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F220" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="H220" s="7"/>
       <c r="K220" s="8"/>
@@ -8988,13 +9009,13 @@
         <v>220</v>
       </c>
       <c r="D221" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E221" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F221" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="H221" s="7"/>
       <c r="K221" s="8"/>
@@ -9014,13 +9035,13 @@
         <v>221</v>
       </c>
       <c r="D222" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E222" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F222" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="H222" s="7"/>
       <c r="K222" s="8"/>
@@ -9040,13 +9061,13 @@
         <v>222</v>
       </c>
       <c r="D223" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E223" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F223" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="H223" s="7"/>
       <c r="K223" s="8"/>
@@ -9066,13 +9087,13 @@
         <v>223</v>
       </c>
       <c r="D224" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E224" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F224" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H224" s="7"/>
       <c r="K224" s="8"/>
@@ -9092,13 +9113,13 @@
         <v>224</v>
       </c>
       <c r="D225" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E225" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="F225" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="H225" s="7"/>
       <c r="K225" s="8"/>
@@ -9118,13 +9139,13 @@
         <v>225</v>
       </c>
       <c r="D226" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E226" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F226" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="H226" s="7" t="n">
         <v>21</v>
@@ -9133,10 +9154,10 @@
         <v>85</v>
       </c>
       <c r="J226" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="K226" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="L226" s="7"/>
       <c r="N226" s="8"/>
@@ -9154,13 +9175,13 @@
         <v>226</v>
       </c>
       <c r="D227" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E227" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F227" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="H227" s="7" t="n">
         <v>22</v>
@@ -9169,10 +9190,10 @@
         <v>85</v>
       </c>
       <c r="J227" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="K227" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="L227" s="7"/>
       <c r="N227" s="8"/>
@@ -9190,13 +9211,13 @@
         <v>227</v>
       </c>
       <c r="D228" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E228" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F228" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="H228" s="7"/>
       <c r="K228" s="8"/>
@@ -9216,13 +9237,13 @@
         <v>228</v>
       </c>
       <c r="D229" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E229" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F229" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="H229" s="7"/>
       <c r="K229" s="8"/>
@@ -9242,13 +9263,13 @@
         <v>229</v>
       </c>
       <c r="D230" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E230" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F230" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H230" s="7"/>
       <c r="K230" s="8"/>
@@ -9268,13 +9289,13 @@
         <v>230</v>
       </c>
       <c r="D231" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E231" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F231" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H231" s="7"/>
       <c r="K231" s="8"/>
@@ -9294,13 +9315,13 @@
         <v>231</v>
       </c>
       <c r="D232" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E232" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F232" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="H232" s="7"/>
       <c r="K232" s="8"/>
@@ -9320,13 +9341,13 @@
         <v>232</v>
       </c>
       <c r="D233" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E233" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F233" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H233" s="7"/>
       <c r="K233" s="8"/>
@@ -9346,13 +9367,13 @@
         <v>233</v>
       </c>
       <c r="D234" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E234" s="2" t="s">
         <v>158</v>
       </c>
       <c r="F234" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H234" s="7"/>
       <c r="K234" s="8"/>
@@ -9372,13 +9393,13 @@
         <v>234</v>
       </c>
       <c r="D235" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E235" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="F235" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="H235" s="7"/>
       <c r="K235" s="8"/>
@@ -9398,13 +9419,13 @@
         <v>235</v>
       </c>
       <c r="D236" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E236" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F236" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="H236" s="7"/>
       <c r="K236" s="8"/>
@@ -9424,13 +9445,13 @@
         <v>236</v>
       </c>
       <c r="D237" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E237" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F237" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="H237" s="7"/>
       <c r="K237" s="8"/>
@@ -9450,13 +9471,13 @@
         <v>237</v>
       </c>
       <c r="D238" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E238" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F238" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="H238" s="7"/>
       <c r="K238" s="8"/>
@@ -9476,13 +9497,13 @@
         <v>238</v>
       </c>
       <c r="D239" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E239" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F239" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="H239" s="7"/>
       <c r="K239" s="8"/>
@@ -9502,13 +9523,13 @@
         <v>239</v>
       </c>
       <c r="D240" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E240" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F240" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="H240" s="7"/>
       <c r="K240" s="8"/>
@@ -9528,13 +9549,13 @@
         <v>240</v>
       </c>
       <c r="D241" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F241" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="H241" s="7"/>
       <c r="K241" s="8"/>
@@ -9554,13 +9575,13 @@
         <v>241</v>
       </c>
       <c r="D242" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E242" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="H242" s="7"/>
       <c r="K242" s="8"/>
@@ -9580,13 +9601,13 @@
         <v>242</v>
       </c>
       <c r="D243" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E243" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F243" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="H243" s="7"/>
       <c r="K243" s="8"/>
@@ -9607,32 +9628,32 @@
       </c>
       <c r="H244" s="7"/>
       <c r="J244" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="K244" s="8"/>
       <c r="L244" s="7"/>
       <c r="M244" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="N244" s="8"/>
       <c r="O244" s="7"/>
       <c r="P244" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="Q244" s="8"/>
       <c r="R244" s="7"/>
       <c r="S244" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="T244" s="8"/>
       <c r="U244" s="7"/>
       <c r="V244" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="W244" s="8"/>
       <c r="X244" s="7"/>
       <c r="Y244" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="Z244" s="8"/>
     </row>
@@ -9653,7 +9674,7 @@
       <c r="X245" s="7"/>
       <c r="Z245" s="8"/>
     </row>
-    <row r="246" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="246" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="n">
         <v>245</v>
       </c>
@@ -9664,14 +9685,14 @@
         <v>59</v>
       </c>
       <c r="J246" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="K246" s="8"/>
       <c r="L246" s="7" t="n">
         <v>26</v>
       </c>
       <c r="M246" s="2" t="s">
-        <v>539</v>
+        <v>344</v>
       </c>
       <c r="N246" s="8"/>
       <c r="O246" s="7" t="n">
@@ -9695,12 +9716,8 @@
         <v>542</v>
       </c>
       <c r="W246" s="8"/>
-      <c r="X246" s="7" t="n">
-        <v>26</v>
-      </c>
-      <c r="Y246" s="2" t="s">
-        <v>539</v>
-      </c>
+      <c r="X246" s="0"/>
+      <c r="Y246" s="0"/>
       <c r="Z246" s="8"/>
     </row>
     <row r="247" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10050,23 +10067,61 @@
       <c r="X261" s="7"/>
       <c r="Z261" s="8"/>
     </row>
-    <row r="262" s="11" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="262" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="10"/>
+      <c r="B262" s="9"/>
+      <c r="C262" s="9"/>
+      <c r="D262" s="9"/>
+      <c r="E262" s="9"/>
+      <c r="F262" s="9"/>
+      <c r="G262" s="9"/>
       <c r="H262" s="10"/>
+      <c r="I262" s="9"/>
+      <c r="J262" s="9"/>
+      <c r="K262" s="9"/>
       <c r="L262" s="10"/>
+      <c r="M262" s="9"/>
+      <c r="N262" s="9"/>
       <c r="O262" s="10"/>
+      <c r="P262" s="9"/>
+      <c r="Q262" s="9"/>
       <c r="R262" s="10"/>
+      <c r="S262" s="9"/>
+      <c r="T262" s="9"/>
       <c r="U262" s="10"/>
+      <c r="V262" s="9"/>
+      <c r="W262" s="9"/>
       <c r="X262" s="10"/>
-    </row>
-    <row r="263" s="11" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y262" s="9"/>
+      <c r="Z262" s="9"/>
+    </row>
+    <row r="263" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="10"/>
+      <c r="B263" s="9"/>
+      <c r="C263" s="9"/>
+      <c r="D263" s="9"/>
+      <c r="E263" s="9"/>
+      <c r="F263" s="9"/>
+      <c r="G263" s="9"/>
       <c r="H263" s="10"/>
+      <c r="I263" s="9"/>
+      <c r="J263" s="9"/>
+      <c r="K263" s="9"/>
       <c r="L263" s="10"/>
+      <c r="M263" s="9"/>
+      <c r="N263" s="9"/>
       <c r="O263" s="10"/>
+      <c r="P263" s="9"/>
+      <c r="Q263" s="9"/>
       <c r="R263" s="10"/>
+      <c r="S263" s="9"/>
+      <c r="T263" s="9"/>
       <c r="U263" s="10"/>
+      <c r="V263" s="9"/>
+      <c r="W263" s="9"/>
       <c r="X263" s="10"/>
+      <c r="Y263" s="9"/>
+      <c r="Z263" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Z269"/>
@@ -10092,7 +10147,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="X142:Y142 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10119,131 +10174,131 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12"/>
+      <c r="A1" s="11"/>
       <c r="B1" s="4"/>
       <c r="C1" s="6" t="s">
         <v>557</v>
       </c>
       <c r="D1" s="4"/>
-      <c r="E1" s="12"/>
+      <c r="E1" s="11"/>
       <c r="F1" s="6" t="s">
         <v>558</v>
       </c>
       <c r="G1" s="4"/>
-      <c r="H1" s="12"/>
+      <c r="H1" s="11"/>
       <c r="I1" s="6" t="s">
         <v>559</v>
       </c>
       <c r="J1" s="4"/>
-      <c r="K1" s="12"/>
+      <c r="K1" s="11"/>
       <c r="L1" s="6" t="s">
         <v>560</v>
       </c>
       <c r="M1" s="4"/>
-      <c r="N1" s="12"/>
+      <c r="N1" s="11"/>
       <c r="O1" s="6" t="s">
         <v>561</v>
       </c>
       <c r="P1" s="4"/>
-      <c r="Q1" s="12"/>
+      <c r="Q1" s="11"/>
       <c r="R1" s="6" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12"/>
+      <c r="A2" s="11"/>
       <c r="C2" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="K2" s="12"/>
+      <c r="K2" s="11"/>
       <c r="L2" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="N2" s="12"/>
+      <c r="N2" s="11"/>
       <c r="O2" s="8" t="s">
         <v>563</v>
       </c>
-      <c r="Q2" s="12"/>
+      <c r="Q2" s="11"/>
       <c r="R2" s="8" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12"/>
+      <c r="A3" s="11"/>
       <c r="C3" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="H3" s="12"/>
+      <c r="H3" s="11"/>
       <c r="I3" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="K3" s="12"/>
+      <c r="K3" s="11"/>
       <c r="L3" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="N3" s="12"/>
+      <c r="N3" s="11"/>
       <c r="O3" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="Q3" s="12"/>
+      <c r="Q3" s="11"/>
       <c r="R3" s="8" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12"/>
+      <c r="A4" s="11"/>
       <c r="C4" s="8" t="s">
         <v>565</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="8" t="s">
         <v>566</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="K4" s="12"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="8" t="s">
         <v>568</v>
       </c>
-      <c r="N4" s="12"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="8" t="s">
         <v>569</v>
       </c>
-      <c r="Q4" s="12"/>
+      <c r="Q4" s="11"/>
       <c r="R4" s="8" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
+      <c r="A5" s="11"/>
       <c r="C5" s="8"/>
-      <c r="E5" s="12"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="8"/>
-      <c r="H5" s="12"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="8"/>
-      <c r="K5" s="12"/>
+      <c r="K5" s="11"/>
       <c r="L5" s="8"/>
-      <c r="N5" s="12"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="8"/>
-      <c r="Q5" s="12"/>
+      <c r="Q5" s="11"/>
       <c r="R5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
+      <c r="A6" s="11" t="n">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -10252,31 +10307,31 @@
       <c r="C6" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="12" t="n">
+      <c r="E6" s="11" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="12" t="n">
+      <c r="H6" s="11" t="n">
         <v>1</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="K6" s="12" t="n">
+      <c r="K6" s="11" t="n">
         <v>1</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>541</v>
       </c>
-      <c r="N6" s="12" t="n">
+      <c r="N6" s="11" t="n">
         <v>1</v>
       </c>
       <c r="O6" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="Q6" s="12" t="n">
+      <c r="Q6" s="11" t="n">
         <v>1</v>
       </c>
       <c r="R6" s="8" t="s">
@@ -10284,7 +10339,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="n">
+      <c r="A7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -10293,31 +10348,31 @@
       <c r="C7" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="12" t="n">
+      <c r="E7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="H7" s="12" t="n">
+      <c r="H7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="K7" s="12" t="n">
+      <c r="K7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="N7" s="12" t="n">
+      <c r="N7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="O7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="Q7" s="12" t="n">
+      <c r="Q7" s="11" t="n">
         <v>2</v>
       </c>
       <c r="R7" s="8" t="s">
@@ -10325,7 +10380,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="n">
+      <c r="A8" s="11" t="n">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -10334,31 +10389,31 @@
       <c r="C8" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="12" t="n">
+      <c r="E8" s="11" t="n">
         <v>3</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="H8" s="11" t="n">
         <v>3</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>546</v>
       </c>
-      <c r="K8" s="12" t="n">
+      <c r="K8" s="11" t="n">
         <v>3</v>
       </c>
       <c r="L8" s="8" t="s">
         <v>546</v>
       </c>
-      <c r="N8" s="12" t="n">
+      <c r="N8" s="11" t="n">
         <v>3</v>
       </c>
       <c r="O8" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="Q8" s="12" t="n">
+      <c r="Q8" s="11" t="n">
         <v>3</v>
       </c>
       <c r="R8" s="8" t="s">
@@ -10366,7 +10421,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
+      <c r="A9" s="11" t="n">
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -10375,31 +10430,31 @@
       <c r="C9" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="E9" s="12" t="n">
+      <c r="E9" s="11" t="n">
         <v>4</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="12" t="n">
+      <c r="H9" s="11" t="n">
         <v>4</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="12" t="n">
+      <c r="K9" s="11" t="n">
         <v>4</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="12" t="n">
+      <c r="N9" s="11" t="n">
         <v>4</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="Q9" s="12" t="n">
+      <c r="Q9" s="11" t="n">
         <v>4</v>
       </c>
       <c r="R9" s="8" t="s">
@@ -10407,7 +10462,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="n">
+      <c r="A10" s="11" t="n">
         <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -10416,31 +10471,31 @@
       <c r="C10" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="12" t="n">
+      <c r="E10" s="11" t="n">
         <v>5</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="12" t="n">
+      <c r="H10" s="11" t="n">
         <v>5</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="K10" s="12" t="n">
+      <c r="K10" s="11" t="n">
         <v>5</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="N10" s="12" t="n">
+      <c r="N10" s="11" t="n">
         <v>5</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="Q10" s="12" t="n">
+      <c r="Q10" s="11" t="n">
         <v>5</v>
       </c>
       <c r="R10" s="8" t="s">
@@ -10448,7 +10503,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="n">
+      <c r="A11" s="11" t="n">
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -10457,31 +10512,31 @@
       <c r="C11" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="E11" s="12" t="n">
+      <c r="E11" s="11" t="n">
         <v>6</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="12" t="n">
+      <c r="H11" s="11" t="n">
         <v>6</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="K11" s="12" t="n">
+      <c r="K11" s="11" t="n">
         <v>6</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="N11" s="12" t="n">
+      <c r="N11" s="11" t="n">
         <v>6</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="Q11" s="12" t="n">
+      <c r="Q11" s="11" t="n">
         <v>6</v>
       </c>
       <c r="R11" s="8" t="s">
@@ -10489,7 +10544,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="n">
+      <c r="A12" s="11" t="n">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -10498,31 +10553,31 @@
       <c r="C12" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="E12" s="12" t="n">
+      <c r="E12" s="11" t="n">
         <v>7</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="H12" s="12" t="n">
+      <c r="H12" s="11" t="n">
         <v>7</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="K12" s="12" t="n">
+      <c r="K12" s="11" t="n">
         <v>7</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="N12" s="12" t="n">
+      <c r="N12" s="11" t="n">
         <v>7</v>
       </c>
       <c r="O12" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="Q12" s="12" t="n">
+      <c r="Q12" s="11" t="n">
         <v>7</v>
       </c>
       <c r="R12" s="8" t="s">
@@ -10530,7 +10585,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="n">
+      <c r="A13" s="11" t="n">
         <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -10539,31 +10594,31 @@
       <c r="C13" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E13" s="12" t="n">
+      <c r="E13" s="11" t="n">
         <v>8</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="H13" s="12" t="n">
+      <c r="H13" s="11" t="n">
         <v>8</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="K13" s="12" t="n">
+      <c r="K13" s="11" t="n">
         <v>8</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="N13" s="12" t="n">
+      <c r="N13" s="11" t="n">
         <v>8</v>
       </c>
       <c r="O13" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="Q13" s="12" t="n">
+      <c r="Q13" s="11" t="n">
         <v>8</v>
       </c>
       <c r="R13" s="8" t="s">
@@ -10571,7 +10626,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="n">
+      <c r="A14" s="11" t="n">
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -10580,31 +10635,31 @@
       <c r="C14" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E14" s="12" t="n">
+      <c r="E14" s="11" t="n">
         <v>9</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="H14" s="12" t="n">
+      <c r="H14" s="11" t="n">
         <v>9</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="K14" s="12" t="n">
+      <c r="K14" s="11" t="n">
         <v>9</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="N14" s="12" t="n">
+      <c r="N14" s="11" t="n">
         <v>9</v>
       </c>
       <c r="O14" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="Q14" s="12" t="n">
+      <c r="Q14" s="11" t="n">
         <v>9</v>
       </c>
       <c r="R14" s="8" t="s">
@@ -10612,40 +10667,40 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="n">
+      <c r="A15" s="11" t="n">
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>571</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="E15" s="12" t="n">
+        <v>539</v>
+      </c>
+      <c r="E15" s="11" t="n">
         <v>10</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="H15" s="12" t="n">
+      <c r="H15" s="11" t="n">
         <v>10</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="K15" s="12" t="n">
+      <c r="K15" s="11" t="n">
         <v>10</v>
       </c>
       <c r="L15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="N15" s="12" t="n">
+      <c r="N15" s="11" t="n">
         <v>10</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="Q15" s="12" t="n">
+      <c r="Q15" s="11" t="n">
         <v>10</v>
       </c>
       <c r="R15" s="8" t="s">
@@ -10653,7 +10708,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="n">
+      <c r="A16" s="11" t="n">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -10662,31 +10717,31 @@
       <c r="C16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="12" t="n">
+      <c r="E16" s="11" t="n">
         <v>11</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="H16" s="12" t="n">
+      <c r="H16" s="11" t="n">
         <v>11</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="12" t="n">
+      <c r="K16" s="11" t="n">
         <v>11</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="N16" s="12" t="n">
+      <c r="N16" s="11" t="n">
         <v>11</v>
       </c>
       <c r="O16" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="Q16" s="12" t="n">
+      <c r="Q16" s="11" t="n">
         <v>11</v>
       </c>
       <c r="R16" s="8" t="s">
@@ -10694,7 +10749,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="n">
+      <c r="A17" s="11" t="n">
         <v>12</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -10703,31 +10758,31 @@
       <c r="C17" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="E17" s="12" t="n">
+      <c r="E17" s="11" t="n">
         <v>12</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="H17" s="12" t="n">
+      <c r="H17" s="11" t="n">
         <v>12</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="K17" s="12" t="n">
+      <c r="K17" s="11" t="n">
         <v>12</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="N17" s="12" t="n">
+      <c r="N17" s="11" t="n">
         <v>12</v>
       </c>
       <c r="O17" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="Q17" s="12" t="n">
+      <c r="Q17" s="11" t="n">
         <v>12</v>
       </c>
       <c r="R17" s="8" t="s">
@@ -10735,7 +10790,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12" t="n">
+      <c r="A18" s="11" t="n">
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -10744,31 +10799,31 @@
       <c r="C18" s="8" t="s">
         <v>335</v>
       </c>
-      <c r="E18" s="12" t="n">
+      <c r="E18" s="11" t="n">
         <v>13</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>310</v>
       </c>
-      <c r="H18" s="12" t="n">
+      <c r="H18" s="11" t="n">
         <v>13</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="K18" s="12" t="n">
+      <c r="K18" s="11" t="n">
         <v>13</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="N18" s="12" t="n">
+      <c r="N18" s="11" t="n">
         <v>13</v>
       </c>
       <c r="O18" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="Q18" s="12" t="n">
+      <c r="Q18" s="11" t="n">
         <v>13</v>
       </c>
       <c r="R18" s="8" t="s">
@@ -10776,7 +10831,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="n">
+      <c r="A19" s="11" t="n">
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -10785,31 +10840,31 @@
       <c r="C19" s="8" t="s">
         <v>585</v>
       </c>
-      <c r="E19" s="12" t="n">
+      <c r="E19" s="11" t="n">
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="H19" s="12" t="n">
+      <c r="H19" s="11" t="n">
         <v>14</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="12" t="n">
+      <c r="K19" s="11" t="n">
         <v>14</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="N19" s="12" t="n">
+      <c r="N19" s="11" t="n">
         <v>14</v>
       </c>
       <c r="O19" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="Q19" s="12" t="n">
+      <c r="Q19" s="11" t="n">
         <v>14</v>
       </c>
       <c r="R19" s="8" t="s">
@@ -10817,40 +10872,40 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="n">
+      <c r="A20" s="11" t="n">
         <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>582</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="E20" s="12" t="n">
+        <v>363</v>
+      </c>
+      <c r="E20" s="11" t="n">
         <v>15</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="H20" s="12" t="n">
+      <c r="H20" s="11" t="n">
         <v>15</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="K20" s="12" t="n">
+      <c r="K20" s="11" t="n">
         <v>15</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="N20" s="12" t="n">
+      <c r="N20" s="11" t="n">
         <v>15</v>
       </c>
       <c r="O20" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="Q20" s="12" t="n">
+      <c r="Q20" s="11" t="n">
         <v>15</v>
       </c>
       <c r="R20" s="8" t="s">
@@ -10858,7 +10913,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="n">
+      <c r="A21" s="11" t="n">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -10867,31 +10922,31 @@
       <c r="C21" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="E21" s="12" t="n">
+      <c r="E21" s="11" t="n">
         <v>16</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="H21" s="12" t="n">
+      <c r="H21" s="11" t="n">
         <v>16</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K21" s="12" t="n">
+      <c r="K21" s="11" t="n">
         <v>16</v>
       </c>
       <c r="L21" s="8" t="s">
         <v>588</v>
       </c>
-      <c r="N21" s="12" t="n">
+      <c r="N21" s="11" t="n">
         <v>16</v>
       </c>
       <c r="O21" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="Q21" s="12" t="n">
+      <c r="Q21" s="11" t="n">
         <v>16</v>
       </c>
       <c r="R21" s="8" t="s">
@@ -10899,7 +10954,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="n">
+      <c r="A22" s="11" t="n">
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -10908,31 +10963,31 @@
       <c r="C22" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="E22" s="12" t="n">
+      <c r="E22" s="11" t="n">
         <v>17</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="H22" s="12" t="n">
+      <c r="H22" s="11" t="n">
         <v>17</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="K22" s="12" t="n">
+      <c r="K22" s="11" t="n">
         <v>17</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="N22" s="12" t="n">
+      <c r="N22" s="11" t="n">
         <v>17</v>
       </c>
       <c r="O22" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="Q22" s="12" t="n">
+      <c r="Q22" s="11" t="n">
         <v>17</v>
       </c>
       <c r="R22" s="8" t="s">
@@ -10940,40 +10995,40 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="n">
+      <c r="A23" s="11" t="n">
         <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>591</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="E23" s="12" t="n">
+        <v>406</v>
+      </c>
+      <c r="E23" s="11" t="n">
         <v>18</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="H23" s="12" t="n">
+        <v>374</v>
+      </c>
+      <c r="H23" s="11" t="n">
         <v>18</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="K23" s="12" t="n">
+      <c r="K23" s="11" t="n">
         <v>18</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>296</v>
       </c>
-      <c r="N23" s="12" t="n">
+      <c r="N23" s="11" t="n">
         <v>18</v>
       </c>
       <c r="O23" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="Q23" s="12" t="n">
+      <c r="Q23" s="11" t="n">
         <v>18</v>
       </c>
       <c r="R23" s="8" t="s">
@@ -10981,7 +11036,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="n">
+      <c r="A24" s="11" t="n">
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -10990,31 +11045,31 @@
       <c r="C24" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="E24" s="12" t="n">
+      <c r="E24" s="11" t="n">
         <v>19</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="H24" s="12" t="n">
+      <c r="H24" s="11" t="n">
         <v>19</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="K24" s="12" t="n">
+      <c r="K24" s="11" t="n">
         <v>19</v>
       </c>
       <c r="L24" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="N24" s="12" t="n">
+      <c r="N24" s="11" t="n">
         <v>19</v>
       </c>
       <c r="O24" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="Q24" s="12" t="n">
+      <c r="Q24" s="11" t="n">
         <v>19</v>
       </c>
       <c r="R24" s="8" t="s">
@@ -11022,7 +11077,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="n">
+      <c r="A25" s="11" t="n">
         <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -11031,31 +11086,31 @@
       <c r="C25" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="E25" s="12" t="n">
+      <c r="E25" s="11" t="n">
         <v>20</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="H25" s="12" t="n">
+      <c r="H25" s="11" t="n">
         <v>20</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="K25" s="12" t="n">
+      <c r="K25" s="11" t="n">
         <v>20</v>
       </c>
       <c r="L25" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="N25" s="12" t="n">
+      <c r="N25" s="11" t="n">
         <v>20</v>
       </c>
       <c r="O25" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="Q25" s="12" t="n">
+      <c r="Q25" s="11" t="n">
         <v>20</v>
       </c>
       <c r="R25" s="8" t="s">
@@ -11063,40 +11118,40 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="n">
+      <c r="A26" s="11" t="n">
         <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>591</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="E26" s="12" t="n">
+        <v>506</v>
+      </c>
+      <c r="E26" s="11" t="n">
         <v>21</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="H26" s="12" t="n">
+      <c r="H26" s="11" t="n">
         <v>21</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="K26" s="12" t="n">
+      <c r="K26" s="11" t="n">
         <v>21</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="N26" s="12" t="n">
+      <c r="N26" s="11" t="n">
         <v>21</v>
       </c>
       <c r="O26" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="Q26" s="12" t="n">
+      <c r="Q26" s="11" t="n">
         <v>21</v>
       </c>
       <c r="R26" s="8" t="s">
@@ -11104,40 +11159,40 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="n">
+      <c r="A27" s="11" t="n">
         <v>22</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>591</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="E27" s="12" t="n">
+        <v>510</v>
+      </c>
+      <c r="E27" s="11" t="n">
         <v>22</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="H27" s="12" t="n">
+        <v>411</v>
+      </c>
+      <c r="H27" s="11" t="n">
         <v>22</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="K27" s="12" t="n">
+      <c r="K27" s="11" t="n">
         <v>22</v>
       </c>
       <c r="L27" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="N27" s="12" t="n">
+      <c r="N27" s="11" t="n">
         <v>22</v>
       </c>
       <c r="O27" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="Q27" s="12" t="n">
+      <c r="Q27" s="11" t="n">
         <v>22</v>
       </c>
       <c r="R27" s="8" t="s">
@@ -11145,7 +11200,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="n">
+      <c r="A28" s="11" t="n">
         <v>23</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -11154,19 +11209,19 @@
       <c r="C28" s="8" t="s">
         <v>543</v>
       </c>
-      <c r="E28" s="12" t="n">
+      <c r="E28" s="11" t="n">
         <v>23</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="K28" s="12" t="n">
+      <c r="K28" s="11" t="n">
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="Q28" s="12" t="n">
+      <c r="Q28" s="11" t="n">
         <v>23</v>
       </c>
       <c r="R28" s="8" t="s">
@@ -11174,7 +11229,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="n">
+      <c r="A29" s="11" t="n">
         <v>24</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -11183,19 +11238,19 @@
       <c r="C29" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="E29" s="12" t="n">
+      <c r="E29" s="11" t="n">
         <v>24</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K29" s="12" t="n">
+      <c r="K29" s="11" t="n">
         <v>24</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="Q29" s="12" t="n">
+      <c r="Q29" s="11" t="n">
         <v>24</v>
       </c>
       <c r="R29" s="8" t="s">
@@ -11203,7 +11258,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="n">
+      <c r="A30" s="11" t="n">
         <v>25</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -11212,19 +11267,19 @@
       <c r="C30" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="E30" s="12" t="n">
+      <c r="E30" s="11" t="n">
         <v>25</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="K30" s="12" t="n">
+      <c r="K30" s="11" t="n">
         <v>25</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="Q30" s="12" t="n">
+      <c r="Q30" s="11" t="n">
         <v>25</v>
       </c>
       <c r="R30" s="8" t="s">
@@ -11232,7 +11287,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="n">
+      <c r="A31" s="11" t="n">
         <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -11241,19 +11296,19 @@
       <c r="C31" s="8" t="s">
         <v>550</v>
       </c>
-      <c r="E31" s="12" t="n">
+      <c r="E31" s="11" t="n">
         <v>26</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>539</v>
-      </c>
-      <c r="K31" s="12" t="n">
+        <v>344</v>
+      </c>
+      <c r="K31" s="11" t="n">
         <v>26</v>
       </c>
       <c r="L31" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="Q31" s="12" t="n">
+      <c r="Q31" s="11" t="n">
         <v>26</v>
       </c>
       <c r="R31" s="8" t="s">
@@ -11261,7 +11316,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="n">
+      <c r="A32" s="11" t="n">
         <v>27</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -11270,19 +11325,19 @@
       <c r="C32" s="8" t="s">
         <v>552</v>
       </c>
-      <c r="E32" s="12" t="n">
+      <c r="E32" s="11" t="n">
         <v>27</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="K32" s="12" t="n">
+        <v>367</v>
+      </c>
+      <c r="K32" s="11" t="n">
         <v>27</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="Q32" s="12" t="n">
+      <c r="Q32" s="11" t="n">
         <v>27</v>
       </c>
       <c r="R32" s="8" t="s">
@@ -11290,7 +11345,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="n">
+      <c r="A33" s="11" t="n">
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -11299,19 +11354,19 @@
       <c r="C33" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E33" s="12" t="n">
+      <c r="E33" s="11" t="n">
         <v>28</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="K33" s="12" t="n">
+      <c r="K33" s="11" t="n">
         <v>28</v>
       </c>
       <c r="L33" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="Q33" s="12" t="n">
+      <c r="Q33" s="11" t="n">
         <v>28</v>
       </c>
       <c r="R33" s="8" t="s">
@@ -11319,27 +11374,27 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="12" t="n">
+      <c r="E34" s="11" t="n">
         <v>29</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="K34" s="12" t="n">
+        <v>360</v>
+      </c>
+      <c r="K34" s="11" t="n">
         <v>29</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="12" t="n">
+      <c r="E35" s="11" t="n">
         <v>30</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="K35" s="12" t="n">
+        <v>364</v>
+      </c>
+      <c r="K35" s="11" t="n">
         <v>30</v>
       </c>
       <c r="L35" s="8" t="s">
@@ -11347,13 +11402,13 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="12" t="n">
+      <c r="E36" s="11" t="n">
         <v>31</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="K36" s="12" t="n">
+      <c r="K36" s="11" t="n">
         <v>31</v>
       </c>
       <c r="L36" s="8" t="s">
@@ -11361,13 +11416,13 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="12" t="n">
+      <c r="E37" s="11" t="n">
         <v>32</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="K37" s="12" t="n">
+      <c r="K37" s="11" t="n">
         <v>32</v>
       </c>
       <c r="L37" s="8" t="s">
@@ -11375,7 +11430,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K38" s="12" t="n">
+      <c r="K38" s="11" t="n">
         <v>33</v>
       </c>
       <c r="L38" s="8" t="s">

</xml_diff>